<commit_message>
type(doc) : Mise à jour de la planification initale
[45min][Done]
</commit_message>
<xml_diff>
--- a/Doc/planification/Planification_initiale.xlsx
+++ b/Doc/planification/Planification_initiale.xlsx
@@ -8,13 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pg66hua\Documents\GitHub\GitJournal\Doc\planification\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D44A7EED-63DC-49F0-8B16-B694396ADD34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF1E0730-6B5F-4A9A-AD80-9C2CC81D8CF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-240" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planification Initale" sheetId="2" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
+    <sheet name="Diagram de Gantt" sheetId="3" r:id="rId2"/>
+    <sheet name="calendrier" sheetId="4" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="77">
   <si>
     <t>Sprint 1</t>
   </si>
@@ -127,6 +129,147 @@
   </si>
   <si>
     <t>+</t>
+  </si>
+  <si>
+    <t>Après Midi</t>
+  </si>
+  <si>
+    <t>28.04 - 02.05</t>
+  </si>
+  <si>
+    <t>05.05 - 09.05</t>
+  </si>
+  <si>
+    <t>12.05 - 16.05</t>
+  </si>
+  <si>
+    <t>19.05 - 23.05</t>
+  </si>
+  <si>
+    <t>26.05 - 30.05</t>
+  </si>
+  <si>
+    <t>02.06 - 06.06</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Absences - imprévus </t>
+  </si>
+  <si>
+    <t>Analyse - Planification initiale</t>
+  </si>
+  <si>
+    <t>Autre - Imprévus</t>
+  </si>
+  <si>
+    <t>Doc - Journal de travail</t>
+  </si>
+  <si>
+    <t>Doc - Rapport</t>
+  </si>
+  <si>
+    <t>Informer - Recherche des thèmes et compétences demandées</t>
+  </si>
+  <si>
+    <t>Informer - Recherches internet, documentation, forums</t>
+  </si>
+  <si>
+    <t>Meeting - Chef de Projet</t>
+  </si>
+  <si>
+    <t>Meeting - Expert</t>
+  </si>
+  <si>
+    <t>Planifier - Mise en place de la méthode de gestion du projet</t>
+  </si>
+  <si>
+    <t>Planifier - Mise en place des tâches</t>
+  </si>
+  <si>
+    <t>Réalisation - Interfaces</t>
+  </si>
+  <si>
+    <t>Réaliser - Déboguages</t>
+  </si>
+  <si>
+    <t>Réaliser - Mise en place de l'environnement de travail</t>
+  </si>
+  <si>
+    <t>Réaliser - Programmation</t>
+  </si>
+  <si>
+    <t>tacheplus - creation de la release et du mail aux Experts</t>
+  </si>
+  <si>
+    <t>tacheplus - test</t>
+  </si>
+  <si>
+    <t>Tester - Test des fonctionnalités</t>
+  </si>
+  <si>
+    <t>Nom</t>
+  </si>
+  <si>
+    <t>Objectifs</t>
+  </si>
+  <si>
+    <t>Durée</t>
+  </si>
+  <si>
+    <t>Dates</t>
+  </si>
+  <si>
+    <t>Date Sprint Review</t>
+  </si>
+  <si>
+    <t>Férié</t>
+  </si>
+  <si>
+    <t>Examens</t>
+  </si>
+  <si>
+    <t>05.05.2025 au 16.05.2025</t>
+  </si>
+  <si>
+    <t>05.19.2025 au 02.06.2025</t>
+  </si>
+  <si>
+    <t>vendredi 23.05.2025 à 9H00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Donner son Token à l'app </t>
+  </si>
+  <si>
+    <t>Documentation</t>
+  </si>
+  <si>
+    <t>~8H</t>
+  </si>
+  <si>
+    <t>~10H50</t>
+  </si>
+  <si>
+    <t>~18H</t>
+  </si>
+  <si>
+    <t>~2H</t>
+  </si>
+  <si>
+    <t>~10H</t>
+  </si>
+  <si>
+    <t>~12H</t>
+  </si>
+  <si>
+    <t>~10H30</t>
+  </si>
+  <si>
+    <t>05:35</t>
+  </si>
+  <si>
+    <t>03:10</t>
+  </si>
+  <si>
+    <t>07:15</t>
   </si>
 </sst>
 </file>
@@ -136,7 +279,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -144,8 +287,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="11">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -206,8 +362,26 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="30">
+  <borders count="64">
     <border>
       <left/>
       <right/>
@@ -576,11 +750,429 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="hair">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="hair">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="hair">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="hair">
+        <color indexed="64"/>
+      </top>
+      <bottom style="hair">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="hair">
+        <color indexed="64"/>
+      </top>
+      <bottom style="hair">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="hair">
+        <color indexed="64"/>
+      </top>
+      <bottom style="hair">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="hair">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="hair">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="hair">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="hair">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="hair">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="hair">
+        <color indexed="64"/>
+      </top>
+      <bottom style="hair">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="hair">
+        <color indexed="64"/>
+      </top>
+      <bottom style="hair">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="hair">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="hair">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="hair">
+        <color indexed="64"/>
+      </top>
+      <bottom style="hair">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="hair">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="hair">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="hair">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="hair">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="hair">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="hair">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="hair">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="hair">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="hair">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="hair">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="hair">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="hair">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="68">
+  <cellXfs count="158">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
@@ -598,126 +1190,17 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="27" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="26" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="36" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="38" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -736,6 +1219,12 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="14" fontId="0" fillId="4" borderId="28" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -745,9 +1234,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -760,14 +1246,378 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="54" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="53" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="48" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="49" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="47" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="46" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="47" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="48" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="38" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="39" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="39" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="42" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="35" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="41" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="42" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="39" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="56" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="38" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="39" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="41" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="42" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="21" fontId="0" fillId="11" borderId="55" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="21" fontId="0" fillId="11" borderId="39" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="21" fontId="0" fillId="11" borderId="41" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="21" fontId="0" fillId="11" borderId="38" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="21" fontId="0" fillId="11" borderId="35" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="57" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="58" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="59" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="60" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="61" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="62" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="63" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="37" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="21" fontId="0" fillId="11" borderId="55" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="35" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="36" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="11" borderId="55" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="11" borderId="56" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="11" borderId="55" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="6" borderId="37" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="11" borderId="35" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="36" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="38" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="39" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="39" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="11" borderId="38" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="11" borderId="39" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="38" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="11" borderId="39" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="6" borderId="38" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="6" borderId="39" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="11" borderId="41" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="11" borderId="42" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="6" borderId="41" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="6" borderId="42" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="41" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="42" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1049,10 +1899,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2164D50-CA97-486F-9059-303E28D57A6D}">
-  <dimension ref="B2:L33"/>
+  <dimension ref="B2:R33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L24" sqref="L24:L25"/>
+      <selection activeCell="F37" sqref="F37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1064,304 +1914,415 @@
     <col min="7" max="7" width="4.7109375" style="3" customWidth="1"/>
     <col min="8" max="8" width="11.42578125" style="3" customWidth="1"/>
     <col min="9" max="11" width="9.42578125" style="3" customWidth="1"/>
-    <col min="12" max="16384" width="11.42578125" style="3"/>
+    <col min="12" max="13" width="11.42578125" style="3"/>
+    <col min="14" max="14" width="18.28515625" style="3" customWidth="1"/>
+    <col min="15" max="15" width="34" style="3" customWidth="1"/>
+    <col min="16" max="16" width="8.28515625" style="3" customWidth="1"/>
+    <col min="17" max="17" width="34" style="3" customWidth="1"/>
+    <col min="18" max="18" width="8.28515625" style="3" customWidth="1"/>
+    <col min="19" max="16384" width="11.42578125" style="3"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B2" s="49" t="s">
+    <row r="2" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="66" t="s">
+      <c r="C2" s="35" t="s">
         <v>19</v>
       </c>
-      <c r="D2" s="66"/>
-      <c r="E2" s="66"/>
-      <c r="F2" s="66"/>
-      <c r="H2" s="49" t="s">
+      <c r="D2" s="35"/>
+      <c r="E2" s="35"/>
+      <c r="F2" s="35"/>
+      <c r="H2" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="I2" s="66" t="s">
+      <c r="I2" s="35" t="s">
         <v>20</v>
       </c>
-      <c r="J2" s="66"/>
-      <c r="K2" s="66"/>
-      <c r="L2" s="66"/>
-    </row>
-    <row r="3" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B3" s="49"/>
-      <c r="C3" s="66"/>
-      <c r="D3" s="66"/>
-      <c r="E3" s="66"/>
-      <c r="F3" s="66"/>
-      <c r="H3" s="49"/>
-      <c r="I3" s="66"/>
-      <c r="J3" s="66"/>
-      <c r="K3" s="66"/>
-      <c r="L3" s="66"/>
-    </row>
-    <row r="4" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="J2" s="35"/>
+      <c r="K2" s="35"/>
+      <c r="L2" s="35"/>
+    </row>
+    <row r="3" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B3" s="25"/>
+      <c r="C3" s="35"/>
+      <c r="D3" s="35"/>
+      <c r="E3" s="35"/>
+      <c r="F3" s="35"/>
+      <c r="H3" s="25"/>
+      <c r="I3" s="35"/>
+      <c r="J3" s="35"/>
+      <c r="K3" s="35"/>
+      <c r="L3" s="35"/>
+      <c r="N3" s="112" t="s">
+        <v>55</v>
+      </c>
+      <c r="O3" s="113" t="s">
+        <v>0</v>
+      </c>
+      <c r="P3" s="114"/>
+      <c r="Q3" s="115" t="s">
+        <v>1</v>
+      </c>
+      <c r="R3" s="116"/>
+    </row>
+    <row r="4" spans="2:18" x14ac:dyDescent="0.25">
       <c r="G4" s="4"/>
       <c r="H4" s="4"/>
-    </row>
-    <row r="5" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B5" s="65" t="s">
+      <c r="N4" s="117" t="s">
+        <v>56</v>
+      </c>
+      <c r="O4" s="118" t="s">
+        <v>65</v>
+      </c>
+      <c r="P4" s="132" t="s">
+        <v>70</v>
+      </c>
+      <c r="Q4" s="119" t="s">
+        <v>26</v>
+      </c>
+      <c r="R4" s="131" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="5" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B5" s="34" t="s">
         <v>25</v>
       </c>
-      <c r="C5" s="65"/>
-      <c r="D5" s="65"/>
-      <c r="E5" s="65"/>
-      <c r="F5" s="65"/>
-      <c r="H5" s="65" t="s">
+      <c r="C5" s="34"/>
+      <c r="D5" s="34"/>
+      <c r="E5" s="34"/>
+      <c r="F5" s="34"/>
+      <c r="H5" s="34" t="s">
         <v>25</v>
       </c>
-      <c r="I5" s="65"/>
-      <c r="J5" s="65"/>
-      <c r="K5" s="65"/>
-      <c r="L5" s="65"/>
-    </row>
-    <row r="6" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B6" s="60" t="s">
+      <c r="I5" s="34"/>
+      <c r="J5" s="34"/>
+      <c r="K5" s="34"/>
+      <c r="L5" s="34"/>
+      <c r="N5" s="120"/>
+      <c r="O5" s="118" t="s">
+        <v>5</v>
+      </c>
+      <c r="P5" s="132" t="s">
+        <v>73</v>
+      </c>
+      <c r="Q5" s="119" t="s">
+        <v>17</v>
+      </c>
+      <c r="R5" s="131" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="6" spans="2:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="36" t="s">
         <v>24</v>
       </c>
-      <c r="C6" s="60"/>
-      <c r="D6" s="60"/>
-      <c r="E6" s="60"/>
-      <c r="F6" s="60"/>
-      <c r="H6" s="60" t="s">
+      <c r="C6" s="36"/>
+      <c r="D6" s="36"/>
+      <c r="E6" s="36"/>
+      <c r="F6" s="36"/>
+      <c r="H6" s="36" t="s">
         <v>28</v>
       </c>
-      <c r="I6" s="60"/>
-      <c r="J6" s="60"/>
-      <c r="K6" s="60"/>
-      <c r="L6" s="60"/>
-    </row>
-    <row r="7" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B7" s="60"/>
-      <c r="C7" s="60"/>
-      <c r="D7" s="60"/>
-      <c r="E7" s="60"/>
-      <c r="F7" s="60"/>
-      <c r="H7" s="60"/>
-      <c r="I7" s="60"/>
-      <c r="J7" s="60"/>
-      <c r="K7" s="60"/>
-      <c r="L7" s="60"/>
-    </row>
-    <row r="9" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B9" s="63" t="s">
+      <c r="I6" s="36"/>
+      <c r="J6" s="36"/>
+      <c r="K6" s="36"/>
+      <c r="L6" s="36"/>
+      <c r="N6" s="120"/>
+      <c r="O6" s="118" t="s">
+        <v>4</v>
+      </c>
+      <c r="P6" s="132" t="s">
+        <v>72</v>
+      </c>
+      <c r="Q6" s="121"/>
+      <c r="R6" s="131"/>
+    </row>
+    <row r="7" spans="2:18" ht="30" x14ac:dyDescent="0.25">
+      <c r="B7" s="36"/>
+      <c r="C7" s="36"/>
+      <c r="D7" s="36"/>
+      <c r="E7" s="36"/>
+      <c r="F7" s="36"/>
+      <c r="H7" s="36"/>
+      <c r="I7" s="36"/>
+      <c r="J7" s="36"/>
+      <c r="K7" s="36"/>
+      <c r="L7" s="36"/>
+      <c r="N7" s="120"/>
+      <c r="O7" s="118" t="s">
+        <v>16</v>
+      </c>
+      <c r="P7" s="132" t="s">
+        <v>71</v>
+      </c>
+      <c r="Q7" s="121"/>
+      <c r="R7" s="131"/>
+    </row>
+    <row r="8" spans="2:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="N8" s="120"/>
+      <c r="O8" s="118" t="s">
+        <v>66</v>
+      </c>
+      <c r="P8" s="132" t="s">
+        <v>71</v>
+      </c>
+      <c r="Q8" s="118" t="s">
+        <v>66</v>
+      </c>
+      <c r="R8" s="131" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="9" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B9" s="31" t="s">
         <v>27</v>
       </c>
-      <c r="C9" s="63"/>
-      <c r="D9" s="63"/>
-      <c r="E9" s="63"/>
-      <c r="F9" s="63"/>
+      <c r="C9" s="31"/>
+      <c r="D9" s="31"/>
+      <c r="E9" s="31"/>
+      <c r="F9" s="31"/>
       <c r="G9" s="4"/>
-      <c r="H9" s="63" t="s">
+      <c r="H9" s="31" t="s">
         <v>27</v>
       </c>
-      <c r="I9" s="63"/>
-      <c r="J9" s="63"/>
-      <c r="K9" s="63"/>
-      <c r="L9" s="63"/>
-    </row>
-    <row r="10" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B10" s="64" t="s">
+      <c r="I9" s="31"/>
+      <c r="J9" s="31"/>
+      <c r="K9" s="31"/>
+      <c r="L9" s="31"/>
+      <c r="N9" s="117" t="s">
+        <v>57</v>
+      </c>
+      <c r="O9" s="122" t="s">
+        <v>24</v>
+      </c>
+      <c r="P9" s="123"/>
+      <c r="Q9" s="124" t="s">
+        <v>28</v>
+      </c>
+      <c r="R9" s="125"/>
+    </row>
+    <row r="10" spans="2:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="32" t="s">
         <v>21</v>
       </c>
-      <c r="C10" s="64"/>
-      <c r="D10" s="64"/>
-      <c r="E10" s="64"/>
-      <c r="F10" s="64"/>
+      <c r="C10" s="32"/>
+      <c r="D10" s="32"/>
+      <c r="E10" s="32"/>
+      <c r="F10" s="32"/>
       <c r="G10" s="4"/>
-      <c r="H10" s="64" t="s">
+      <c r="H10" s="32" t="s">
         <v>22</v>
       </c>
-      <c r="I10" s="64"/>
-      <c r="J10" s="64"/>
-      <c r="K10" s="64"/>
-      <c r="L10" s="64"/>
-    </row>
-    <row r="11" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B11" s="64"/>
-      <c r="C11" s="64"/>
-      <c r="D11" s="64"/>
-      <c r="E11" s="64"/>
-      <c r="F11" s="64"/>
+      <c r="I10" s="32"/>
+      <c r="J10" s="32"/>
+      <c r="K10" s="32"/>
+      <c r="L10" s="32"/>
+      <c r="N10" s="117" t="s">
+        <v>58</v>
+      </c>
+      <c r="O10" s="122" t="s">
+        <v>62</v>
+      </c>
+      <c r="P10" s="123"/>
+      <c r="Q10" s="124" t="s">
+        <v>63</v>
+      </c>
+      <c r="R10" s="125"/>
+    </row>
+    <row r="11" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="32"/>
+      <c r="C11" s="32"/>
+      <c r="D11" s="32"/>
+      <c r="E11" s="32"/>
+      <c r="F11" s="32"/>
       <c r="G11" s="4"/>
-      <c r="H11" s="64"/>
-      <c r="I11" s="64"/>
-      <c r="J11" s="64"/>
-      <c r="K11" s="64"/>
-      <c r="L11" s="64"/>
-    </row>
-    <row r="12" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="H11" s="32"/>
+      <c r="I11" s="32"/>
+      <c r="J11" s="32"/>
+      <c r="K11" s="32"/>
+      <c r="L11" s="32"/>
+      <c r="N11" s="126" t="s">
+        <v>59</v>
+      </c>
+      <c r="O11" s="127" t="s">
+        <v>62</v>
+      </c>
+      <c r="P11" s="128"/>
+      <c r="Q11" s="129" t="s">
+        <v>64</v>
+      </c>
+      <c r="R11" s="130"/>
+    </row>
+    <row r="12" spans="2:18" x14ac:dyDescent="0.25">
       <c r="G12" s="4"/>
     </row>
-    <row r="13" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B13" s="67" t="s">
+    <row r="13" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B13" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="C13" s="67"/>
-      <c r="D13" s="67"/>
-      <c r="E13" s="67"/>
-      <c r="F13" s="67"/>
+      <c r="C13" s="33"/>
+      <c r="D13" s="33"/>
+      <c r="E13" s="33"/>
+      <c r="F13" s="33"/>
       <c r="G13" s="4"/>
-      <c r="H13" s="67" t="s">
+      <c r="H13" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="I13" s="67"/>
-      <c r="J13" s="67"/>
-      <c r="K13" s="67"/>
-      <c r="L13" s="67"/>
-    </row>
-    <row r="14" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B14" s="62" t="s">
+      <c r="I13" s="33"/>
+      <c r="J13" s="33"/>
+      <c r="K13" s="33"/>
+      <c r="L13" s="33"/>
+    </row>
+    <row r="14" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B14" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="C14" s="62"/>
-      <c r="D14" s="62"/>
-      <c r="E14" s="62"/>
-      <c r="F14" s="62"/>
+      <c r="C14" s="30"/>
+      <c r="D14" s="30"/>
+      <c r="E14" s="30"/>
+      <c r="F14" s="30"/>
       <c r="G14" s="4"/>
-      <c r="H14" s="62" t="s">
+      <c r="H14" s="30" t="s">
         <v>26</v>
       </c>
-      <c r="I14" s="62"/>
-      <c r="J14" s="62"/>
-      <c r="K14" s="62"/>
-      <c r="L14" s="62"/>
-    </row>
-    <row r="15" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B15" s="62"/>
-      <c r="C15" s="62"/>
-      <c r="D15" s="62"/>
-      <c r="E15" s="62"/>
-      <c r="F15" s="62"/>
+      <c r="I14" s="30"/>
+      <c r="J14" s="30"/>
+      <c r="K14" s="30"/>
+      <c r="L14" s="30"/>
+    </row>
+    <row r="15" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B15" s="30"/>
+      <c r="C15" s="30"/>
+      <c r="D15" s="30"/>
+      <c r="E15" s="30"/>
+      <c r="F15" s="30"/>
       <c r="G15" s="4"/>
-      <c r="H15" s="62"/>
-      <c r="I15" s="62"/>
-      <c r="J15" s="62"/>
-      <c r="K15" s="62"/>
-      <c r="L15" s="62"/>
-    </row>
-    <row r="16" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B16" s="61" t="s">
+      <c r="H15" s="30"/>
+      <c r="I15" s="30"/>
+      <c r="J15" s="30"/>
+      <c r="K15" s="30"/>
+      <c r="L15" s="30"/>
+    </row>
+    <row r="16" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B16" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="C16" s="62"/>
-      <c r="D16" s="62"/>
-      <c r="E16" s="62"/>
-      <c r="F16" s="62"/>
+      <c r="C16" s="30"/>
+      <c r="D16" s="30"/>
+      <c r="E16" s="30"/>
+      <c r="F16" s="30"/>
       <c r="G16" s="4"/>
-      <c r="H16" s="61" t="s">
+      <c r="H16" s="29" t="s">
         <v>17</v>
       </c>
-      <c r="I16" s="62"/>
-      <c r="J16" s="62"/>
-      <c r="K16" s="62"/>
-      <c r="L16" s="62"/>
+      <c r="I16" s="30"/>
+      <c r="J16" s="30"/>
+      <c r="K16" s="30"/>
+      <c r="L16" s="30"/>
     </row>
     <row r="17" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B17" s="62"/>
-      <c r="C17" s="62"/>
-      <c r="D17" s="62"/>
-      <c r="E17" s="62"/>
-      <c r="F17" s="62"/>
+      <c r="B17" s="30"/>
+      <c r="C17" s="30"/>
+      <c r="D17" s="30"/>
+      <c r="E17" s="30"/>
+      <c r="F17" s="30"/>
       <c r="G17" s="4"/>
-      <c r="H17" s="62"/>
-      <c r="I17" s="62"/>
-      <c r="J17" s="62"/>
-      <c r="K17" s="62"/>
-      <c r="L17" s="62"/>
+      <c r="H17" s="30"/>
+      <c r="I17" s="30"/>
+      <c r="J17" s="30"/>
+      <c r="K17" s="30"/>
+      <c r="L17" s="30"/>
     </row>
     <row r="18" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B18" s="61" t="s">
+      <c r="B18" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="C18" s="62"/>
-      <c r="D18" s="62"/>
-      <c r="E18" s="62"/>
-      <c r="F18" s="62"/>
+      <c r="C18" s="30"/>
+      <c r="D18" s="30"/>
+      <c r="E18" s="30"/>
+      <c r="F18" s="30"/>
       <c r="G18" s="4"/>
-      <c r="H18" s="61"/>
-      <c r="I18" s="62"/>
-      <c r="J18" s="62"/>
-      <c r="K18" s="62"/>
-      <c r="L18" s="62"/>
+      <c r="H18" s="29"/>
+      <c r="I18" s="30"/>
+      <c r="J18" s="30"/>
+      <c r="K18" s="30"/>
+      <c r="L18" s="30"/>
     </row>
     <row r="19" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B19" s="62"/>
-      <c r="C19" s="62"/>
-      <c r="D19" s="62"/>
-      <c r="E19" s="62"/>
-      <c r="F19" s="62"/>
+      <c r="B19" s="30"/>
+      <c r="C19" s="30"/>
+      <c r="D19" s="30"/>
+      <c r="E19" s="30"/>
+      <c r="F19" s="30"/>
       <c r="G19" s="4"/>
-      <c r="H19" s="62"/>
-      <c r="I19" s="62"/>
-      <c r="J19" s="62"/>
-      <c r="K19" s="62"/>
-      <c r="L19" s="62"/>
+      <c r="H19" s="30"/>
+      <c r="I19" s="30"/>
+      <c r="J19" s="30"/>
+      <c r="K19" s="30"/>
+      <c r="L19" s="30"/>
     </row>
     <row r="20" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B20" s="61" t="s">
+      <c r="B20" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="C20" s="62"/>
-      <c r="D20" s="62"/>
-      <c r="E20" s="62"/>
-      <c r="F20" s="62"/>
-      <c r="H20" s="61"/>
-      <c r="I20" s="62"/>
-      <c r="J20" s="62"/>
-      <c r="K20" s="62"/>
-      <c r="L20" s="62"/>
+      <c r="C20" s="30"/>
+      <c r="D20" s="30"/>
+      <c r="E20" s="30"/>
+      <c r="F20" s="30"/>
+      <c r="H20" s="29"/>
+      <c r="I20" s="30"/>
+      <c r="J20" s="30"/>
+      <c r="K20" s="30"/>
+      <c r="L20" s="30"/>
     </row>
     <row r="21" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B21" s="62"/>
-      <c r="C21" s="62"/>
-      <c r="D21" s="62"/>
-      <c r="E21" s="62"/>
-      <c r="F21" s="62"/>
-      <c r="H21" s="62"/>
-      <c r="I21" s="62"/>
-      <c r="J21" s="62"/>
-      <c r="K21" s="62"/>
-      <c r="L21" s="62"/>
+      <c r="B21" s="30"/>
+      <c r="C21" s="30"/>
+      <c r="D21" s="30"/>
+      <c r="E21" s="30"/>
+      <c r="F21" s="30"/>
+      <c r="H21" s="30"/>
+      <c r="I21" s="30"/>
+      <c r="J21" s="30"/>
+      <c r="K21" s="30"/>
+      <c r="L21" s="30"/>
     </row>
     <row r="23" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="24" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B24" s="57">
+      <c r="B24" s="26">
         <v>45782</v>
       </c>
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
       <c r="E24" s="1"/>
-      <c r="F24" s="57">
+      <c r="F24" s="26">
         <v>45793</v>
       </c>
       <c r="G24" s="8"/>
-      <c r="H24" s="57">
+      <c r="H24" s="26">
         <v>45796</v>
       </c>
       <c r="I24" s="1"/>
       <c r="J24" s="1"/>
       <c r="K24" s="1"/>
-      <c r="L24" s="57">
+      <c r="L24" s="26">
         <v>45810</v>
       </c>
     </row>
     <row r="25" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="58"/>
+      <c r="B25" s="27"/>
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>
-      <c r="F25" s="58"/>
+      <c r="F25" s="27"/>
       <c r="G25" s="8"/>
-      <c r="H25" s="58"/>
+      <c r="H25" s="27"/>
       <c r="I25" s="1"/>
       <c r="J25" s="1"/>
       <c r="K25" s="1"/>
-      <c r="L25" s="58"/>
+      <c r="L25" s="27"/>
     </row>
     <row r="26" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B26" s="2"/>
@@ -1403,38 +2364,38 @@
       <c r="L28" s="10"/>
     </row>
     <row r="29" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B29" s="48" t="s">
+      <c r="B29" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="C29" s="49"/>
-      <c r="D29" s="49"/>
-      <c r="E29" s="49"/>
-      <c r="F29" s="59" t="s">
+      <c r="C29" s="25"/>
+      <c r="D29" s="25"/>
+      <c r="E29" s="25"/>
+      <c r="F29" s="28" t="s">
         <v>18</v>
       </c>
       <c r="G29" s="8"/>
-      <c r="H29" s="48" t="s">
+      <c r="H29" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="I29" s="49"/>
-      <c r="J29" s="49"/>
-      <c r="K29" s="49"/>
-      <c r="L29" s="59" t="s">
+      <c r="I29" s="25"/>
+      <c r="J29" s="25"/>
+      <c r="K29" s="25"/>
+      <c r="L29" s="28" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="30" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="48"/>
-      <c r="C30" s="49"/>
-      <c r="D30" s="49"/>
-      <c r="E30" s="49"/>
-      <c r="F30" s="59"/>
+      <c r="B30" s="24"/>
+      <c r="C30" s="25"/>
+      <c r="D30" s="25"/>
+      <c r="E30" s="25"/>
+      <c r="F30" s="28"/>
       <c r="G30" s="8"/>
-      <c r="H30" s="48"/>
-      <c r="I30" s="49"/>
-      <c r="J30" s="49"/>
-      <c r="K30" s="49"/>
-      <c r="L30" s="59"/>
+      <c r="H30" s="24"/>
+      <c r="I30" s="25"/>
+      <c r="J30" s="25"/>
+      <c r="K30" s="25"/>
+      <c r="L30" s="28"/>
     </row>
     <row r="31" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B31" s="1"/>
@@ -1456,13 +2417,13 @@
       <c r="E32" s="1"/>
       <c r="F32" s="1"/>
       <c r="G32" s="8"/>
-      <c r="H32" s="51" t="s">
+      <c r="H32" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="I32" s="52"/>
-      <c r="J32" s="52"/>
-      <c r="K32" s="52"/>
-      <c r="L32" s="53"/>
+      <c r="I32" s="19"/>
+      <c r="J32" s="19"/>
+      <c r="K32" s="19"/>
+      <c r="L32" s="20"/>
     </row>
     <row r="33" spans="2:12" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B33" s="1"/>
@@ -1471,14 +2432,22 @@
       <c r="E33" s="1"/>
       <c r="F33" s="1"/>
       <c r="G33" s="8"/>
-      <c r="H33" s="54"/>
-      <c r="I33" s="55"/>
-      <c r="J33" s="55"/>
-      <c r="K33" s="55"/>
-      <c r="L33" s="56"/>
+      <c r="H33" s="21"/>
+      <c r="I33" s="22"/>
+      <c r="J33" s="22"/>
+      <c r="K33" s="22"/>
+      <c r="L33" s="23"/>
     </row>
   </sheetData>
-  <mergeCells count="31">
+  <mergeCells count="39">
+    <mergeCell ref="O3:P3"/>
+    <mergeCell ref="O9:P9"/>
+    <mergeCell ref="O11:P11"/>
+    <mergeCell ref="Q3:R3"/>
+    <mergeCell ref="Q11:R11"/>
+    <mergeCell ref="Q10:R10"/>
+    <mergeCell ref="Q9:R9"/>
+    <mergeCell ref="O10:P10"/>
     <mergeCell ref="H5:L5"/>
     <mergeCell ref="B9:F9"/>
     <mergeCell ref="B10:F11"/>
@@ -1517,53 +2486,1532 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16CE2A06-A4CD-4B66-AA78-4E5ADC2697C1}">
+  <dimension ref="B2:N39"/>
+  <sheetViews>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J18" sqref="J18:J19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="28.28515625" customWidth="1"/>
+    <col min="3" max="14" width="15.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C3" s="51" t="s">
+        <v>31</v>
+      </c>
+      <c r="D3" s="52"/>
+      <c r="E3" s="51" t="s">
+        <v>32</v>
+      </c>
+      <c r="F3" s="52"/>
+      <c r="G3" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="H3" s="52"/>
+      <c r="I3" s="51" t="s">
+        <v>34</v>
+      </c>
+      <c r="J3" s="52"/>
+      <c r="K3" s="51" t="s">
+        <v>35</v>
+      </c>
+      <c r="L3" s="52"/>
+      <c r="M3" s="51" t="s">
+        <v>36</v>
+      </c>
+      <c r="N3" s="52"/>
+    </row>
+    <row r="4" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B4" s="50" t="s">
+        <v>37</v>
+      </c>
+      <c r="C4" s="42"/>
+      <c r="D4" s="44"/>
+      <c r="E4" s="42"/>
+      <c r="F4" s="44"/>
+      <c r="G4" s="42"/>
+      <c r="H4" s="44"/>
+      <c r="I4" s="42"/>
+      <c r="J4" s="44"/>
+      <c r="K4" s="42"/>
+      <c r="L4" s="44"/>
+      <c r="M4" s="42"/>
+      <c r="N4" s="44"/>
+    </row>
+    <row r="5" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B5" s="48"/>
+      <c r="C5" s="43"/>
+      <c r="D5" s="39"/>
+      <c r="E5" s="43"/>
+      <c r="F5" s="39"/>
+      <c r="G5" s="43"/>
+      <c r="H5" s="39"/>
+      <c r="I5" s="43"/>
+      <c r="J5" s="39"/>
+      <c r="K5" s="43"/>
+      <c r="L5" s="39"/>
+      <c r="M5" s="43"/>
+      <c r="N5" s="39"/>
+    </row>
+    <row r="6" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B6" s="47" t="s">
+        <v>38</v>
+      </c>
+      <c r="C6" s="45"/>
+      <c r="D6" s="46"/>
+      <c r="E6" s="45"/>
+      <c r="F6" s="46"/>
+      <c r="G6" s="37"/>
+      <c r="H6" s="39"/>
+      <c r="I6" s="37"/>
+      <c r="J6" s="39"/>
+      <c r="K6" s="37"/>
+      <c r="L6" s="39"/>
+      <c r="M6" s="37"/>
+      <c r="N6" s="39"/>
+    </row>
+    <row r="7" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B7" s="48"/>
+      <c r="C7" s="45"/>
+      <c r="D7" s="46"/>
+      <c r="E7" s="45"/>
+      <c r="F7" s="46"/>
+      <c r="G7" s="38"/>
+      <c r="H7" s="39"/>
+      <c r="I7" s="38"/>
+      <c r="J7" s="39"/>
+      <c r="K7" s="38"/>
+      <c r="L7" s="39"/>
+      <c r="M7" s="38"/>
+      <c r="N7" s="39"/>
+    </row>
+    <row r="8" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B8" s="47" t="s">
+        <v>39</v>
+      </c>
+      <c r="C8" s="37"/>
+      <c r="D8" s="39"/>
+      <c r="E8" s="37"/>
+      <c r="F8" s="39"/>
+      <c r="G8" s="37"/>
+      <c r="H8" s="39"/>
+      <c r="I8" s="37"/>
+      <c r="J8" s="39"/>
+      <c r="K8" s="37"/>
+      <c r="L8" s="39"/>
+      <c r="M8" s="37"/>
+      <c r="N8" s="39"/>
+    </row>
+    <row r="9" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B9" s="47"/>
+      <c r="C9" s="38"/>
+      <c r="D9" s="39"/>
+      <c r="E9" s="38"/>
+      <c r="F9" s="39"/>
+      <c r="G9" s="38"/>
+      <c r="H9" s="39"/>
+      <c r="I9" s="38"/>
+      <c r="J9" s="39"/>
+      <c r="K9" s="38"/>
+      <c r="L9" s="39"/>
+      <c r="M9" s="38"/>
+      <c r="N9" s="39"/>
+    </row>
+    <row r="10" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B10" s="47" t="s">
+        <v>40</v>
+      </c>
+      <c r="C10" s="37"/>
+      <c r="D10" s="39"/>
+      <c r="E10" s="37"/>
+      <c r="F10" s="39"/>
+      <c r="G10" s="37"/>
+      <c r="H10" s="39"/>
+      <c r="I10" s="37"/>
+      <c r="J10" s="39"/>
+      <c r="K10" s="37"/>
+      <c r="L10" s="39"/>
+      <c r="M10" s="37"/>
+      <c r="N10" s="39"/>
+    </row>
+    <row r="11" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B11" s="48"/>
+      <c r="C11" s="38"/>
+      <c r="D11" s="39"/>
+      <c r="E11" s="38"/>
+      <c r="F11" s="39"/>
+      <c r="G11" s="38"/>
+      <c r="H11" s="39"/>
+      <c r="I11" s="38"/>
+      <c r="J11" s="39"/>
+      <c r="K11" s="38"/>
+      <c r="L11" s="39"/>
+      <c r="M11" s="38"/>
+      <c r="N11" s="39"/>
+    </row>
+    <row r="12" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B12" s="47" t="s">
+        <v>41</v>
+      </c>
+      <c r="C12" s="37"/>
+      <c r="D12" s="39"/>
+      <c r="E12" s="37"/>
+      <c r="F12" s="39"/>
+      <c r="G12" s="37"/>
+      <c r="H12" s="39"/>
+      <c r="I12" s="37"/>
+      <c r="J12" s="39"/>
+      <c r="K12" s="37"/>
+      <c r="L12" s="39"/>
+      <c r="M12" s="37"/>
+      <c r="N12" s="39"/>
+    </row>
+    <row r="13" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B13" s="48"/>
+      <c r="C13" s="38"/>
+      <c r="D13" s="39"/>
+      <c r="E13" s="38"/>
+      <c r="F13" s="39"/>
+      <c r="G13" s="38"/>
+      <c r="H13" s="39"/>
+      <c r="I13" s="38"/>
+      <c r="J13" s="39"/>
+      <c r="K13" s="38"/>
+      <c r="L13" s="39"/>
+      <c r="M13" s="38"/>
+      <c r="N13" s="39"/>
+    </row>
+    <row r="14" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B14" s="47" t="s">
+        <v>42</v>
+      </c>
+      <c r="C14" s="37"/>
+      <c r="D14" s="39"/>
+      <c r="E14" s="37"/>
+      <c r="F14" s="39"/>
+      <c r="G14" s="37"/>
+      <c r="H14" s="39"/>
+      <c r="I14" s="37"/>
+      <c r="J14" s="39"/>
+      <c r="K14" s="37"/>
+      <c r="L14" s="39"/>
+      <c r="M14" s="37"/>
+      <c r="N14" s="39"/>
+    </row>
+    <row r="15" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B15" s="48"/>
+      <c r="C15" s="38"/>
+      <c r="D15" s="39"/>
+      <c r="E15" s="38"/>
+      <c r="F15" s="39"/>
+      <c r="G15" s="38"/>
+      <c r="H15" s="39"/>
+      <c r="I15" s="38"/>
+      <c r="J15" s="39"/>
+      <c r="K15" s="38"/>
+      <c r="L15" s="39"/>
+      <c r="M15" s="38"/>
+      <c r="N15" s="39"/>
+    </row>
+    <row r="16" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B16" s="47" t="s">
+        <v>43</v>
+      </c>
+      <c r="C16" s="37"/>
+      <c r="D16" s="39"/>
+      <c r="E16" s="37"/>
+      <c r="F16" s="39"/>
+      <c r="G16" s="37"/>
+      <c r="H16" s="39"/>
+      <c r="I16" s="37"/>
+      <c r="J16" s="39"/>
+      <c r="K16" s="37"/>
+      <c r="L16" s="39"/>
+      <c r="M16" s="37"/>
+      <c r="N16" s="39"/>
+    </row>
+    <row r="17" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B17" s="47"/>
+      <c r="C17" s="38"/>
+      <c r="D17" s="39"/>
+      <c r="E17" s="38"/>
+      <c r="F17" s="39"/>
+      <c r="G17" s="38"/>
+      <c r="H17" s="39"/>
+      <c r="I17" s="38"/>
+      <c r="J17" s="39"/>
+      <c r="K17" s="38"/>
+      <c r="L17" s="39"/>
+      <c r="M17" s="38"/>
+      <c r="N17" s="39"/>
+    </row>
+    <row r="18" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B18" s="47" t="s">
+        <v>44</v>
+      </c>
+      <c r="C18" s="37"/>
+      <c r="D18" s="46"/>
+      <c r="E18" s="37"/>
+      <c r="F18" s="39"/>
+      <c r="G18" s="37"/>
+      <c r="H18" s="39"/>
+      <c r="I18" s="37"/>
+      <c r="J18" s="39"/>
+      <c r="K18" s="37"/>
+      <c r="L18" s="39"/>
+      <c r="M18" s="37"/>
+      <c r="N18" s="39"/>
+    </row>
+    <row r="19" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B19" s="47"/>
+      <c r="C19" s="38"/>
+      <c r="D19" s="46"/>
+      <c r="E19" s="38"/>
+      <c r="F19" s="39"/>
+      <c r="G19" s="38"/>
+      <c r="H19" s="39"/>
+      <c r="I19" s="38"/>
+      <c r="J19" s="39"/>
+      <c r="K19" s="38"/>
+      <c r="L19" s="39"/>
+      <c r="M19" s="38"/>
+      <c r="N19" s="39"/>
+    </row>
+    <row r="20" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B20" s="47" t="s">
+        <v>45</v>
+      </c>
+      <c r="C20" s="37"/>
+      <c r="D20" s="46"/>
+      <c r="E20" s="37"/>
+      <c r="F20" s="39"/>
+      <c r="G20" s="37"/>
+      <c r="H20" s="39"/>
+      <c r="I20" s="37"/>
+      <c r="J20" s="39"/>
+      <c r="K20" s="37"/>
+      <c r="L20" s="39"/>
+      <c r="M20" s="37"/>
+      <c r="N20" s="39"/>
+    </row>
+    <row r="21" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B21" s="48"/>
+      <c r="C21" s="38"/>
+      <c r="D21" s="46"/>
+      <c r="E21" s="38"/>
+      <c r="F21" s="39"/>
+      <c r="G21" s="38"/>
+      <c r="H21" s="39"/>
+      <c r="I21" s="38"/>
+      <c r="J21" s="39"/>
+      <c r="K21" s="38"/>
+      <c r="L21" s="39"/>
+      <c r="M21" s="38"/>
+      <c r="N21" s="39"/>
+    </row>
+    <row r="22" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B22" s="47" t="s">
+        <v>46</v>
+      </c>
+      <c r="C22" s="37"/>
+      <c r="D22" s="39"/>
+      <c r="E22" s="37"/>
+      <c r="F22" s="39"/>
+      <c r="G22" s="37"/>
+      <c r="H22" s="39"/>
+      <c r="I22" s="37"/>
+      <c r="J22" s="39"/>
+      <c r="K22" s="37"/>
+      <c r="L22" s="39"/>
+      <c r="M22" s="37"/>
+      <c r="N22" s="39"/>
+    </row>
+    <row r="23" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B23" s="48"/>
+      <c r="C23" s="38"/>
+      <c r="D23" s="39"/>
+      <c r="E23" s="38"/>
+      <c r="F23" s="39"/>
+      <c r="G23" s="38"/>
+      <c r="H23" s="39"/>
+      <c r="I23" s="38"/>
+      <c r="J23" s="39"/>
+      <c r="K23" s="38"/>
+      <c r="L23" s="39"/>
+      <c r="M23" s="38"/>
+      <c r="N23" s="39"/>
+    </row>
+    <row r="24" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B24" s="47" t="s">
+        <v>47</v>
+      </c>
+      <c r="C24" s="37"/>
+      <c r="D24" s="39"/>
+      <c r="E24" s="37"/>
+      <c r="F24" s="39"/>
+      <c r="G24" s="37"/>
+      <c r="H24" s="39"/>
+      <c r="I24" s="37"/>
+      <c r="J24" s="39"/>
+      <c r="K24" s="37"/>
+      <c r="L24" s="39"/>
+      <c r="M24" s="37"/>
+      <c r="N24" s="39"/>
+    </row>
+    <row r="25" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B25" s="47"/>
+      <c r="C25" s="38"/>
+      <c r="D25" s="39"/>
+      <c r="E25" s="38"/>
+      <c r="F25" s="39"/>
+      <c r="G25" s="38"/>
+      <c r="H25" s="39"/>
+      <c r="I25" s="38"/>
+      <c r="J25" s="39"/>
+      <c r="K25" s="38"/>
+      <c r="L25" s="39"/>
+      <c r="M25" s="38"/>
+      <c r="N25" s="39"/>
+    </row>
+    <row r="26" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B26" s="47" t="s">
+        <v>48</v>
+      </c>
+      <c r="C26" s="37"/>
+      <c r="D26" s="39"/>
+      <c r="E26" s="37"/>
+      <c r="F26" s="39"/>
+      <c r="G26" s="37"/>
+      <c r="H26" s="39"/>
+      <c r="I26" s="37"/>
+      <c r="J26" s="39"/>
+      <c r="K26" s="37"/>
+      <c r="L26" s="39"/>
+      <c r="M26" s="37"/>
+      <c r="N26" s="39"/>
+    </row>
+    <row r="27" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B27" s="48"/>
+      <c r="C27" s="38"/>
+      <c r="D27" s="39"/>
+      <c r="E27" s="38"/>
+      <c r="F27" s="39"/>
+      <c r="G27" s="38"/>
+      <c r="H27" s="39"/>
+      <c r="I27" s="38"/>
+      <c r="J27" s="39"/>
+      <c r="K27" s="38"/>
+      <c r="L27" s="39"/>
+      <c r="M27" s="38"/>
+      <c r="N27" s="39"/>
+    </row>
+    <row r="28" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B28" s="47" t="s">
+        <v>49</v>
+      </c>
+      <c r="C28" s="37"/>
+      <c r="D28" s="39"/>
+      <c r="E28" s="37"/>
+      <c r="F28" s="39"/>
+      <c r="G28" s="37"/>
+      <c r="H28" s="39"/>
+      <c r="I28" s="37"/>
+      <c r="J28" s="39"/>
+      <c r="K28" s="37"/>
+      <c r="L28" s="39"/>
+      <c r="M28" s="37"/>
+      <c r="N28" s="39"/>
+    </row>
+    <row r="29" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B29" s="47"/>
+      <c r="C29" s="38"/>
+      <c r="D29" s="39"/>
+      <c r="E29" s="38"/>
+      <c r="F29" s="39"/>
+      <c r="G29" s="38"/>
+      <c r="H29" s="39"/>
+      <c r="I29" s="38"/>
+      <c r="J29" s="39"/>
+      <c r="K29" s="38"/>
+      <c r="L29" s="39"/>
+      <c r="M29" s="38"/>
+      <c r="N29" s="39"/>
+    </row>
+    <row r="30" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B30" s="47" t="s">
+        <v>50</v>
+      </c>
+      <c r="C30" s="37"/>
+      <c r="D30" s="39"/>
+      <c r="E30" s="37"/>
+      <c r="F30" s="39"/>
+      <c r="G30" s="37"/>
+      <c r="H30" s="39"/>
+      <c r="I30" s="37"/>
+      <c r="J30" s="39"/>
+      <c r="K30" s="37"/>
+      <c r="L30" s="39"/>
+      <c r="M30" s="37"/>
+      <c r="N30" s="39"/>
+    </row>
+    <row r="31" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B31" s="48"/>
+      <c r="C31" s="38"/>
+      <c r="D31" s="39"/>
+      <c r="E31" s="38"/>
+      <c r="F31" s="39"/>
+      <c r="G31" s="38"/>
+      <c r="H31" s="39"/>
+      <c r="I31" s="38"/>
+      <c r="J31" s="39"/>
+      <c r="K31" s="38"/>
+      <c r="L31" s="39"/>
+      <c r="M31" s="38"/>
+      <c r="N31" s="39"/>
+    </row>
+    <row r="32" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B32" s="47" t="s">
+        <v>51</v>
+      </c>
+      <c r="C32" s="37"/>
+      <c r="D32" s="39"/>
+      <c r="E32" s="37"/>
+      <c r="F32" s="39"/>
+      <c r="G32" s="37"/>
+      <c r="H32" s="39"/>
+      <c r="I32" s="37"/>
+      <c r="J32" s="39"/>
+      <c r="K32" s="37"/>
+      <c r="L32" s="39"/>
+      <c r="M32" s="37"/>
+      <c r="N32" s="39"/>
+    </row>
+    <row r="33" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B33" s="47"/>
+      <c r="C33" s="38"/>
+      <c r="D33" s="39"/>
+      <c r="E33" s="38"/>
+      <c r="F33" s="39"/>
+      <c r="G33" s="38"/>
+      <c r="H33" s="39"/>
+      <c r="I33" s="38"/>
+      <c r="J33" s="39"/>
+      <c r="K33" s="38"/>
+      <c r="L33" s="39"/>
+      <c r="M33" s="38"/>
+      <c r="N33" s="39"/>
+    </row>
+    <row r="34" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B34" s="47" t="s">
+        <v>52</v>
+      </c>
+      <c r="C34" s="37"/>
+      <c r="D34" s="39"/>
+      <c r="E34" s="37"/>
+      <c r="F34" s="39"/>
+      <c r="G34" s="37"/>
+      <c r="H34" s="39"/>
+      <c r="I34" s="37"/>
+      <c r="J34" s="39"/>
+      <c r="K34" s="37"/>
+      <c r="L34" s="39"/>
+      <c r="M34" s="37"/>
+      <c r="N34" s="39"/>
+    </row>
+    <row r="35" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B35" s="48"/>
+      <c r="C35" s="38"/>
+      <c r="D35" s="39"/>
+      <c r="E35" s="38"/>
+      <c r="F35" s="39"/>
+      <c r="G35" s="38"/>
+      <c r="H35" s="39"/>
+      <c r="I35" s="38"/>
+      <c r="J35" s="39"/>
+      <c r="K35" s="38"/>
+      <c r="L35" s="39"/>
+      <c r="M35" s="38"/>
+      <c r="N35" s="39"/>
+    </row>
+    <row r="36" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B36" s="47" t="s">
+        <v>53</v>
+      </c>
+      <c r="C36" s="37"/>
+      <c r="D36" s="39"/>
+      <c r="E36" s="37"/>
+      <c r="F36" s="39"/>
+      <c r="G36" s="37"/>
+      <c r="H36" s="39"/>
+      <c r="I36" s="37"/>
+      <c r="J36" s="39"/>
+      <c r="K36" s="37"/>
+      <c r="L36" s="39"/>
+      <c r="M36" s="37"/>
+      <c r="N36" s="39"/>
+    </row>
+    <row r="37" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B37" s="48"/>
+      <c r="C37" s="38"/>
+      <c r="D37" s="39"/>
+      <c r="E37" s="38"/>
+      <c r="F37" s="39"/>
+      <c r="G37" s="38"/>
+      <c r="H37" s="39"/>
+      <c r="I37" s="38"/>
+      <c r="J37" s="39"/>
+      <c r="K37" s="38"/>
+      <c r="L37" s="39"/>
+      <c r="M37" s="38"/>
+      <c r="N37" s="39"/>
+    </row>
+    <row r="38" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B38" s="47" t="s">
+        <v>54</v>
+      </c>
+      <c r="C38" s="37"/>
+      <c r="D38" s="39"/>
+      <c r="E38" s="37"/>
+      <c r="F38" s="39"/>
+      <c r="G38" s="37"/>
+      <c r="H38" s="39"/>
+      <c r="I38" s="37"/>
+      <c r="J38" s="39"/>
+      <c r="K38" s="37"/>
+      <c r="L38" s="39"/>
+      <c r="M38" s="37"/>
+      <c r="N38" s="39"/>
+    </row>
+    <row r="39" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B39" s="49"/>
+      <c r="C39" s="40"/>
+      <c r="D39" s="41"/>
+      <c r="E39" s="40"/>
+      <c r="F39" s="41"/>
+      <c r="G39" s="40"/>
+      <c r="H39" s="41"/>
+      <c r="I39" s="40"/>
+      <c r="J39" s="41"/>
+      <c r="K39" s="40"/>
+      <c r="L39" s="41"/>
+      <c r="M39" s="40"/>
+      <c r="N39" s="41"/>
+    </row>
+  </sheetData>
+  <mergeCells count="240">
+    <mergeCell ref="I3:J3"/>
+    <mergeCell ref="K3:L3"/>
+    <mergeCell ref="M3:N3"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="B28:B29"/>
+    <mergeCell ref="B30:B31"/>
+    <mergeCell ref="B32:B33"/>
+    <mergeCell ref="B34:B35"/>
+    <mergeCell ref="B36:B37"/>
+    <mergeCell ref="B38:B39"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="B20:B21"/>
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="B26:B27"/>
+    <mergeCell ref="K22:K23"/>
+    <mergeCell ref="L22:L23"/>
+    <mergeCell ref="K24:K25"/>
+    <mergeCell ref="L24:L25"/>
+    <mergeCell ref="I26:I27"/>
+    <mergeCell ref="J26:J27"/>
+    <mergeCell ref="I28:I29"/>
+    <mergeCell ref="J28:J29"/>
+    <mergeCell ref="I16:I17"/>
+    <mergeCell ref="J16:J17"/>
+    <mergeCell ref="I18:I19"/>
+    <mergeCell ref="J18:J19"/>
+    <mergeCell ref="C38:C39"/>
+    <mergeCell ref="D38:D39"/>
+    <mergeCell ref="C24:C25"/>
+    <mergeCell ref="D24:D25"/>
+    <mergeCell ref="C26:C27"/>
+    <mergeCell ref="D26:D27"/>
+    <mergeCell ref="C28:C29"/>
+    <mergeCell ref="D28:D29"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="C16:C17"/>
+    <mergeCell ref="D16:D17"/>
+    <mergeCell ref="C18:C19"/>
+    <mergeCell ref="D18:D19"/>
+    <mergeCell ref="C30:C31"/>
+    <mergeCell ref="D30:D31"/>
+    <mergeCell ref="C32:C33"/>
+    <mergeCell ref="D32:D33"/>
+    <mergeCell ref="C20:C21"/>
+    <mergeCell ref="D20:D21"/>
+    <mergeCell ref="C22:C23"/>
+    <mergeCell ref="D22:D23"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="E4:E5"/>
+    <mergeCell ref="F4:F5"/>
+    <mergeCell ref="E6:E7"/>
+    <mergeCell ref="F6:F7"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="F8:F9"/>
+    <mergeCell ref="C34:C35"/>
+    <mergeCell ref="D34:D35"/>
+    <mergeCell ref="C36:C37"/>
+    <mergeCell ref="D36:D37"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="E22:E23"/>
+    <mergeCell ref="F22:F23"/>
+    <mergeCell ref="E24:E25"/>
+    <mergeCell ref="F24:F25"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="E18:E19"/>
+    <mergeCell ref="F18:F19"/>
+    <mergeCell ref="E20:E21"/>
+    <mergeCell ref="F20:F21"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="F10:F11"/>
+    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="F12:F13"/>
+    <mergeCell ref="E14:E15"/>
+    <mergeCell ref="F14:F15"/>
+    <mergeCell ref="E38:E39"/>
+    <mergeCell ref="F38:F39"/>
+    <mergeCell ref="G4:G5"/>
+    <mergeCell ref="H4:H5"/>
+    <mergeCell ref="G6:G7"/>
+    <mergeCell ref="H6:H7"/>
+    <mergeCell ref="G8:G9"/>
+    <mergeCell ref="H8:H9"/>
+    <mergeCell ref="G10:G11"/>
+    <mergeCell ref="H10:H11"/>
+    <mergeCell ref="E32:E33"/>
+    <mergeCell ref="F32:F33"/>
+    <mergeCell ref="E34:E35"/>
+    <mergeCell ref="F34:F35"/>
+    <mergeCell ref="E36:E37"/>
+    <mergeCell ref="F36:F37"/>
+    <mergeCell ref="E26:E27"/>
+    <mergeCell ref="F26:F27"/>
+    <mergeCell ref="E28:E29"/>
+    <mergeCell ref="F28:F29"/>
+    <mergeCell ref="E30:E31"/>
+    <mergeCell ref="F30:F31"/>
+    <mergeCell ref="E16:E17"/>
+    <mergeCell ref="F16:F17"/>
+    <mergeCell ref="G22:G23"/>
+    <mergeCell ref="H22:H23"/>
+    <mergeCell ref="G24:G25"/>
+    <mergeCell ref="H24:H25"/>
+    <mergeCell ref="G26:G27"/>
+    <mergeCell ref="H26:H27"/>
+    <mergeCell ref="G12:G13"/>
+    <mergeCell ref="H12:H13"/>
+    <mergeCell ref="G14:G15"/>
+    <mergeCell ref="H14:H15"/>
+    <mergeCell ref="G16:G17"/>
+    <mergeCell ref="H16:H17"/>
+    <mergeCell ref="G18:G19"/>
+    <mergeCell ref="H18:H19"/>
+    <mergeCell ref="G20:G21"/>
+    <mergeCell ref="H20:H21"/>
+    <mergeCell ref="G34:G35"/>
+    <mergeCell ref="H34:H35"/>
+    <mergeCell ref="G36:G37"/>
+    <mergeCell ref="H36:H37"/>
+    <mergeCell ref="G38:G39"/>
+    <mergeCell ref="H38:H39"/>
+    <mergeCell ref="G28:G29"/>
+    <mergeCell ref="H28:H29"/>
+    <mergeCell ref="G30:G31"/>
+    <mergeCell ref="H30:H31"/>
+    <mergeCell ref="G32:G33"/>
+    <mergeCell ref="H32:H33"/>
+    <mergeCell ref="I12:I13"/>
+    <mergeCell ref="J12:J13"/>
+    <mergeCell ref="I14:I15"/>
+    <mergeCell ref="J14:J15"/>
+    <mergeCell ref="I4:I5"/>
+    <mergeCell ref="J4:J5"/>
+    <mergeCell ref="I6:I7"/>
+    <mergeCell ref="J6:J7"/>
+    <mergeCell ref="I8:I9"/>
+    <mergeCell ref="J8:J9"/>
+    <mergeCell ref="I36:I37"/>
+    <mergeCell ref="J36:J37"/>
+    <mergeCell ref="I38:I39"/>
+    <mergeCell ref="J38:J39"/>
+    <mergeCell ref="K4:K5"/>
+    <mergeCell ref="L4:L5"/>
+    <mergeCell ref="K6:K7"/>
+    <mergeCell ref="L6:L7"/>
+    <mergeCell ref="K8:K9"/>
+    <mergeCell ref="L8:L9"/>
+    <mergeCell ref="I30:I31"/>
+    <mergeCell ref="J30:J31"/>
+    <mergeCell ref="I32:I33"/>
+    <mergeCell ref="J32:J33"/>
+    <mergeCell ref="I34:I35"/>
+    <mergeCell ref="J34:J35"/>
+    <mergeCell ref="I20:I21"/>
+    <mergeCell ref="J20:J21"/>
+    <mergeCell ref="I22:I23"/>
+    <mergeCell ref="J22:J23"/>
+    <mergeCell ref="I24:I25"/>
+    <mergeCell ref="J24:J25"/>
+    <mergeCell ref="I10:I11"/>
+    <mergeCell ref="J10:J11"/>
+    <mergeCell ref="K18:K19"/>
+    <mergeCell ref="L18:L19"/>
+    <mergeCell ref="K20:K21"/>
+    <mergeCell ref="L20:L21"/>
+    <mergeCell ref="K10:K11"/>
+    <mergeCell ref="L10:L11"/>
+    <mergeCell ref="K12:K13"/>
+    <mergeCell ref="L12:L13"/>
+    <mergeCell ref="K14:K15"/>
+    <mergeCell ref="L14:L15"/>
+    <mergeCell ref="K38:K39"/>
+    <mergeCell ref="L38:L39"/>
+    <mergeCell ref="M4:M5"/>
+    <mergeCell ref="N4:N5"/>
+    <mergeCell ref="M6:M7"/>
+    <mergeCell ref="N6:N7"/>
+    <mergeCell ref="M8:M9"/>
+    <mergeCell ref="N8:N9"/>
+    <mergeCell ref="M10:M11"/>
+    <mergeCell ref="N10:N11"/>
+    <mergeCell ref="K32:K33"/>
+    <mergeCell ref="L32:L33"/>
+    <mergeCell ref="K34:K35"/>
+    <mergeCell ref="L34:L35"/>
+    <mergeCell ref="K36:K37"/>
+    <mergeCell ref="L36:L37"/>
+    <mergeCell ref="K26:K27"/>
+    <mergeCell ref="L26:L27"/>
+    <mergeCell ref="K28:K29"/>
+    <mergeCell ref="L28:L29"/>
+    <mergeCell ref="K30:K31"/>
+    <mergeCell ref="L30:L31"/>
+    <mergeCell ref="K16:K17"/>
+    <mergeCell ref="L16:L17"/>
+    <mergeCell ref="M22:M23"/>
+    <mergeCell ref="N22:N23"/>
+    <mergeCell ref="M24:M25"/>
+    <mergeCell ref="N24:N25"/>
+    <mergeCell ref="M26:M27"/>
+    <mergeCell ref="N26:N27"/>
+    <mergeCell ref="M12:M13"/>
+    <mergeCell ref="N12:N13"/>
+    <mergeCell ref="M14:M15"/>
+    <mergeCell ref="N14:N15"/>
+    <mergeCell ref="M16:M17"/>
+    <mergeCell ref="N16:N17"/>
+    <mergeCell ref="M18:M19"/>
+    <mergeCell ref="N18:N19"/>
+    <mergeCell ref="M20:M21"/>
+    <mergeCell ref="N20:N21"/>
+    <mergeCell ref="M34:M35"/>
+    <mergeCell ref="N34:N35"/>
+    <mergeCell ref="M36:M37"/>
+    <mergeCell ref="N36:N37"/>
+    <mergeCell ref="M38:M39"/>
+    <mergeCell ref="N38:N39"/>
+    <mergeCell ref="M28:M29"/>
+    <mergeCell ref="N28:N29"/>
+    <mergeCell ref="M30:M31"/>
+    <mergeCell ref="N30:N31"/>
+    <mergeCell ref="M32:M33"/>
+    <mergeCell ref="N32:N33"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E58BC6FA-FA0D-44D8-9583-DDDC8777C3AA}">
+  <dimension ref="B3:AD29"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P10" sqref="P10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.28515625" customWidth="1"/>
+    <col min="2" max="2" width="9" customWidth="1"/>
+    <col min="3" max="3" width="6.7109375" customWidth="1"/>
+    <col min="4" max="4" width="10.28515625" customWidth="1"/>
+    <col min="5" max="5" width="6.7109375" customWidth="1"/>
+    <col min="6" max="6" width="10.28515625" customWidth="1"/>
+    <col min="7" max="7" width="6.7109375" customWidth="1"/>
+    <col min="8" max="8" width="10.28515625" customWidth="1"/>
+    <col min="9" max="9" width="6.7109375" customWidth="1"/>
+    <col min="10" max="10" width="10.28515625" customWidth="1"/>
+    <col min="11" max="11" width="6.7109375" customWidth="1"/>
+    <col min="12" max="12" width="10.28515625" customWidth="1"/>
+    <col min="13" max="13" width="6.7109375" customWidth="1"/>
+    <col min="14" max="14" width="10.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="C3" s="53" t="s">
+        <v>31</v>
+      </c>
+      <c r="D3" s="54"/>
+      <c r="E3" s="53" t="s">
+        <v>32</v>
+      </c>
+      <c r="F3" s="54"/>
+      <c r="G3" s="53" t="s">
+        <v>33</v>
+      </c>
+      <c r="H3" s="54"/>
+      <c r="I3" s="53" t="s">
+        <v>34</v>
+      </c>
+      <c r="J3" s="54"/>
+      <c r="K3" s="53" t="s">
+        <v>35</v>
+      </c>
+      <c r="L3" s="54"/>
+      <c r="M3" s="53" t="s">
+        <v>36</v>
+      </c>
+      <c r="N3" s="54"/>
+      <c r="S3" s="59" t="s">
+        <v>15</v>
+      </c>
+      <c r="T3" s="60"/>
+      <c r="U3" s="107">
+        <v>0.23263888888888887</v>
+      </c>
+      <c r="V3" s="102"/>
+      <c r="W3" s="107">
+        <v>0.23263888888888887</v>
+      </c>
+      <c r="X3" s="102"/>
+      <c r="Y3" s="107">
+        <v>0.23263888888888887</v>
+      </c>
+      <c r="Z3" s="102"/>
+      <c r="AA3" s="134">
+        <v>0.13194444444444445</v>
+      </c>
+      <c r="AB3" s="133" t="s">
+        <v>61</v>
+      </c>
+      <c r="AC3" s="111">
+        <v>0.13194444444444445</v>
+      </c>
+      <c r="AD3" s="14" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="C4" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="E4" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="G4" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="H4" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="I4" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="J4" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="K4" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="L4" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="M4" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="N4" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="S4" s="55" t="s">
+        <v>15</v>
+      </c>
+      <c r="T4" s="56"/>
+      <c r="U4" s="55" t="s">
+        <v>15</v>
+      </c>
+      <c r="V4" s="101"/>
+      <c r="W4" s="55" t="s">
+        <v>15</v>
+      </c>
+      <c r="X4" s="56"/>
+      <c r="Y4" s="55" t="s">
+        <v>15</v>
+      </c>
+      <c r="Z4" s="56"/>
+      <c r="AA4" s="55" t="s">
+        <v>15</v>
+      </c>
+      <c r="AB4" s="56"/>
+      <c r="AC4" s="55" t="s">
+        <v>15</v>
+      </c>
+      <c r="AD4" s="56"/>
+    </row>
+    <row r="5" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="B5" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="135" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="136"/>
+      <c r="E5" s="137" t="s">
+        <v>74</v>
+      </c>
+      <c r="F5" s="138"/>
+      <c r="G5" s="137" t="s">
+        <v>74</v>
+      </c>
+      <c r="H5" s="138"/>
+      <c r="I5" s="137" t="s">
+        <v>74</v>
+      </c>
+      <c r="J5" s="138"/>
+      <c r="K5" s="139" t="s">
+        <v>75</v>
+      </c>
+      <c r="L5" s="140" t="s">
+        <v>61</v>
+      </c>
+      <c r="M5" s="141" t="s">
+        <v>75</v>
+      </c>
+      <c r="N5" s="142" t="s">
+        <v>15</v>
+      </c>
+      <c r="S5" s="55" t="s">
+        <v>15</v>
+      </c>
+      <c r="T5" s="56"/>
+      <c r="U5" s="110">
+        <v>0.30208333333333331</v>
+      </c>
+      <c r="V5" s="57"/>
+      <c r="W5" s="110">
+        <v>0.30208333333333331</v>
+      </c>
+      <c r="X5" s="57"/>
+      <c r="Y5" s="110">
+        <v>0.30208333333333331</v>
+      </c>
+      <c r="Z5" s="57"/>
+      <c r="AA5" s="110">
+        <v>0.30208333333333331</v>
+      </c>
+      <c r="AB5" s="57"/>
+      <c r="AC5" s="55" t="s">
+        <v>15</v>
+      </c>
+      <c r="AD5" s="56"/>
+    </row>
+    <row r="6" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="B6" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="143" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" s="144"/>
+      <c r="E6" s="143" t="s">
+        <v>15</v>
+      </c>
+      <c r="F6" s="145"/>
+      <c r="G6" s="143" t="s">
+        <v>15</v>
+      </c>
+      <c r="H6" s="144"/>
+      <c r="I6" s="143" t="s">
+        <v>15</v>
+      </c>
+      <c r="J6" s="144"/>
+      <c r="K6" s="143" t="s">
+        <v>15</v>
+      </c>
+      <c r="L6" s="144"/>
+      <c r="M6" s="143" t="s">
+        <v>15</v>
+      </c>
+      <c r="N6" s="144"/>
+      <c r="S6" s="55" t="s">
+        <v>15</v>
+      </c>
+      <c r="T6" s="56"/>
+      <c r="U6" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="V6" s="108">
+        <v>0.13194444444444445</v>
+      </c>
+      <c r="W6" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="X6" s="108">
+        <v>0.13194444444444445</v>
+      </c>
+      <c r="Y6" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="Z6" s="108">
+        <v>0.13194444444444445</v>
+      </c>
+      <c r="AA6" s="103" t="s">
+        <v>60</v>
+      </c>
+      <c r="AB6" s="104"/>
+      <c r="AC6" s="55" t="s">
+        <v>15</v>
+      </c>
+      <c r="AD6" s="56"/>
+    </row>
+    <row r="7" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="B7" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="143" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" s="144"/>
+      <c r="E7" s="146" t="s">
+        <v>76</v>
+      </c>
+      <c r="F7" s="147"/>
+      <c r="G7" s="146" t="s">
+        <v>76</v>
+      </c>
+      <c r="H7" s="147"/>
+      <c r="I7" s="146" t="s">
+        <v>76</v>
+      </c>
+      <c r="J7" s="147"/>
+      <c r="K7" s="146" t="s">
+        <v>76</v>
+      </c>
+      <c r="L7" s="147"/>
+      <c r="M7" s="143" t="s">
+        <v>15</v>
+      </c>
+      <c r="N7" s="144"/>
+      <c r="S7" s="109">
+        <v>0.30208333333333331</v>
+      </c>
+      <c r="T7" s="58"/>
+      <c r="U7" s="109">
+        <v>0.30208333333333331</v>
+      </c>
+      <c r="V7" s="58"/>
+      <c r="W7" s="109">
+        <v>0.30208333333333331</v>
+      </c>
+      <c r="X7" s="58"/>
+      <c r="Y7" s="109">
+        <v>0.30208333333333331</v>
+      </c>
+      <c r="Z7" s="58"/>
+      <c r="AA7" s="105" t="s">
+        <v>60</v>
+      </c>
+      <c r="AB7" s="106"/>
+      <c r="AC7" s="61" t="s">
+        <v>15</v>
+      </c>
+      <c r="AD7" s="62"/>
+    </row>
+    <row r="8" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="B8" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="143" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" s="144"/>
+      <c r="E8" s="148" t="s">
+        <v>15</v>
+      </c>
+      <c r="F8" s="149" t="s">
+        <v>75</v>
+      </c>
+      <c r="G8" s="148" t="s">
+        <v>15</v>
+      </c>
+      <c r="H8" s="149" t="s">
+        <v>75</v>
+      </c>
+      <c r="I8" s="148" t="s">
+        <v>15</v>
+      </c>
+      <c r="J8" s="149" t="s">
+        <v>75</v>
+      </c>
+      <c r="K8" s="150" t="s">
+        <v>60</v>
+      </c>
+      <c r="L8" s="151"/>
+      <c r="M8" s="143" t="s">
+        <v>15</v>
+      </c>
+      <c r="N8" s="144"/>
+    </row>
+    <row r="9" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="B9" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" s="152" t="s">
+        <v>76</v>
+      </c>
+      <c r="D9" s="153"/>
+      <c r="E9" s="152" t="s">
+        <v>76</v>
+      </c>
+      <c r="F9" s="153"/>
+      <c r="G9" s="152" t="s">
+        <v>76</v>
+      </c>
+      <c r="H9" s="153"/>
+      <c r="I9" s="152" t="s">
+        <v>76</v>
+      </c>
+      <c r="J9" s="153"/>
+      <c r="K9" s="154" t="s">
+        <v>60</v>
+      </c>
+      <c r="L9" s="155"/>
+      <c r="M9" s="156" t="s">
+        <v>15</v>
+      </c>
+      <c r="N9" s="157"/>
+    </row>
+    <row r="21" spans="9:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="22" spans="9:20" x14ac:dyDescent="0.25">
+      <c r="I22" s="76"/>
+      <c r="J22" s="77"/>
+      <c r="K22" s="92" t="s">
+        <v>6</v>
+      </c>
+      <c r="L22" s="93"/>
+      <c r="M22" s="93" t="s">
+        <v>7</v>
+      </c>
+      <c r="N22" s="93"/>
+      <c r="O22" s="93" t="s">
+        <v>8</v>
+      </c>
+      <c r="P22" s="93"/>
+      <c r="Q22" s="93" t="s">
+        <v>9</v>
+      </c>
+      <c r="R22" s="93"/>
+      <c r="S22" s="93" t="s">
+        <v>10</v>
+      </c>
+      <c r="T22" s="96"/>
+    </row>
+    <row r="23" spans="9:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I23" s="78"/>
+      <c r="J23" s="79"/>
+      <c r="K23" s="94"/>
+      <c r="L23" s="95"/>
+      <c r="M23" s="95"/>
+      <c r="N23" s="95"/>
+      <c r="O23" s="95"/>
+      <c r="P23" s="95"/>
+      <c r="Q23" s="95"/>
+      <c r="R23" s="95"/>
+      <c r="S23" s="95"/>
+      <c r="T23" s="97"/>
+    </row>
+    <row r="24" spans="9:20" x14ac:dyDescent="0.25">
+      <c r="I24" s="86" t="s">
+        <v>11</v>
+      </c>
+      <c r="J24" s="87"/>
+      <c r="K24" s="100">
+        <v>0.13194444444444445</v>
+      </c>
+      <c r="L24" s="73"/>
+      <c r="M24" s="74"/>
+      <c r="N24" s="74"/>
+      <c r="O24" s="73">
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="P24" s="73"/>
+      <c r="Q24" s="74"/>
+      <c r="R24" s="74"/>
+      <c r="S24" s="73">
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="T24" s="75"/>
+    </row>
+    <row r="25" spans="9:20" x14ac:dyDescent="0.25">
+      <c r="I25" s="82"/>
+      <c r="J25" s="83"/>
+      <c r="K25" s="67"/>
+      <c r="L25" s="65"/>
+      <c r="M25" s="70"/>
+      <c r="N25" s="70"/>
+      <c r="O25" s="65"/>
+      <c r="P25" s="65"/>
+      <c r="Q25" s="70"/>
+      <c r="R25" s="70"/>
+      <c r="S25" s="65"/>
+      <c r="T25" s="66"/>
+    </row>
+    <row r="26" spans="9:20" x14ac:dyDescent="0.25">
+      <c r="I26" s="82" t="s">
+        <v>12</v>
+      </c>
+      <c r="J26" s="83"/>
+      <c r="K26" s="67">
+        <v>0.10069444444444443</v>
+      </c>
+      <c r="L26" s="65"/>
+      <c r="M26" s="70"/>
+      <c r="N26" s="70"/>
+      <c r="O26" s="65">
+        <v>0.13194444444444445</v>
+      </c>
+      <c r="P26" s="65"/>
+      <c r="Q26" s="65">
+        <v>0.13194444444444445</v>
+      </c>
+      <c r="R26" s="65"/>
+      <c r="S26" s="65">
+        <v>0.13194444444444445</v>
+      </c>
+      <c r="T26" s="66"/>
+    </row>
+    <row r="27" spans="9:20" x14ac:dyDescent="0.25">
+      <c r="I27" s="82"/>
+      <c r="J27" s="83"/>
+      <c r="K27" s="67"/>
+      <c r="L27" s="65"/>
+      <c r="M27" s="70"/>
+      <c r="N27" s="70"/>
+      <c r="O27" s="65"/>
+      <c r="P27" s="65"/>
+      <c r="Q27" s="65"/>
+      <c r="R27" s="65"/>
+      <c r="S27" s="65"/>
+      <c r="T27" s="66"/>
+    </row>
+    <row r="28" spans="9:20" x14ac:dyDescent="0.25">
+      <c r="I28" s="82" t="s">
+        <v>13</v>
+      </c>
+      <c r="J28" s="83"/>
+      <c r="K28" s="67">
+        <f>K24+K26</f>
+        <v>0.2326388888888889</v>
+      </c>
+      <c r="L28" s="65"/>
+      <c r="M28" s="70"/>
+      <c r="N28" s="70"/>
+      <c r="O28" s="65">
+        <v>0.30208333333333331</v>
+      </c>
+      <c r="P28" s="65"/>
+      <c r="Q28" s="65">
+        <v>0.13194444444444445</v>
+      </c>
+      <c r="R28" s="65"/>
+      <c r="S28" s="65">
+        <v>0.30208333333333331</v>
+      </c>
+      <c r="T28" s="66"/>
+    </row>
+    <row r="29" spans="9:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I29" s="84"/>
+      <c r="J29" s="85"/>
+      <c r="K29" s="68"/>
+      <c r="L29" s="69"/>
+      <c r="M29" s="71"/>
+      <c r="N29" s="71"/>
+      <c r="O29" s="69"/>
+      <c r="P29" s="69"/>
+      <c r="Q29" s="69"/>
+      <c r="R29" s="69"/>
+      <c r="S29" s="69"/>
+      <c r="T29" s="72"/>
+    </row>
+  </sheetData>
+  <mergeCells count="80">
+    <mergeCell ref="S6:T6"/>
+    <mergeCell ref="AA6:AB6"/>
+    <mergeCell ref="AC6:AD6"/>
+    <mergeCell ref="S7:T7"/>
+    <mergeCell ref="U7:V7"/>
+    <mergeCell ref="W7:X7"/>
+    <mergeCell ref="Y7:Z7"/>
+    <mergeCell ref="AA7:AB7"/>
+    <mergeCell ref="AC7:AD7"/>
+    <mergeCell ref="AA4:AB4"/>
+    <mergeCell ref="AC4:AD4"/>
+    <mergeCell ref="S5:T5"/>
+    <mergeCell ref="U5:V5"/>
+    <mergeCell ref="W5:X5"/>
+    <mergeCell ref="Y5:Z5"/>
+    <mergeCell ref="AA5:AB5"/>
+    <mergeCell ref="AC5:AD5"/>
+    <mergeCell ref="S3:T3"/>
+    <mergeCell ref="U3:V3"/>
+    <mergeCell ref="W3:X3"/>
+    <mergeCell ref="Y3:Z3"/>
+    <mergeCell ref="S4:T4"/>
+    <mergeCell ref="U4:V4"/>
+    <mergeCell ref="W4:X4"/>
+    <mergeCell ref="Y4:Z4"/>
+    <mergeCell ref="S26:T27"/>
+    <mergeCell ref="I28:J29"/>
+    <mergeCell ref="K28:L29"/>
+    <mergeCell ref="M28:N29"/>
+    <mergeCell ref="O28:P29"/>
+    <mergeCell ref="Q28:R29"/>
+    <mergeCell ref="S28:T29"/>
+    <mergeCell ref="I26:J27"/>
+    <mergeCell ref="K26:L27"/>
+    <mergeCell ref="M26:N27"/>
+    <mergeCell ref="O26:P27"/>
+    <mergeCell ref="Q26:R27"/>
+    <mergeCell ref="S22:T23"/>
+    <mergeCell ref="I24:J25"/>
+    <mergeCell ref="K24:L25"/>
+    <mergeCell ref="M24:N25"/>
+    <mergeCell ref="O24:P25"/>
+    <mergeCell ref="Q24:R25"/>
+    <mergeCell ref="S24:T25"/>
+    <mergeCell ref="I22:J23"/>
+    <mergeCell ref="K22:L23"/>
+    <mergeCell ref="M22:N23"/>
+    <mergeCell ref="O22:P23"/>
+    <mergeCell ref="Q22:R23"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="M3:N3"/>
+    <mergeCell ref="M6:N6"/>
+    <mergeCell ref="M7:N7"/>
+    <mergeCell ref="M9:N9"/>
+    <mergeCell ref="M8:N8"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="K3:L3"/>
+    <mergeCell ref="K8:L8"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="I6:J6"/>
+    <mergeCell ref="I7:J7"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="I5:J5"/>
+    <mergeCell ref="I3:J3"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="G9:H9"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="K6:L6"/>
+    <mergeCell ref="K7:L7"/>
+    <mergeCell ref="K9:L9"/>
+    <mergeCell ref="I9:J9"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="C2:X39"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="M22" sqref="M22:N23"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18:N25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="2" spans="5:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="5:18" x14ac:dyDescent="0.25">
-      <c r="E3" s="37">
+      <c r="E3" s="88">
         <v>45782</v>
       </c>
-      <c r="F3" s="38"/>
+      <c r="F3" s="89"/>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
-      <c r="K3" s="37">
+      <c r="K3" s="88">
         <v>45795</v>
       </c>
-      <c r="L3" s="38"/>
+      <c r="L3" s="89"/>
       <c r="M3" s="1"/>
       <c r="N3" s="1"/>
       <c r="O3" s="1"/>
       <c r="P3" s="1"/>
-      <c r="Q3" s="37">
+      <c r="Q3" s="88">
         <v>45810</v>
       </c>
-      <c r="R3" s="38"/>
+      <c r="R3" s="89"/>
     </row>
     <row r="4" spans="5:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E4" s="39"/>
-      <c r="F4" s="40"/>
+      <c r="E4" s="90"/>
+      <c r="F4" s="91"/>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
-      <c r="K4" s="39"/>
-      <c r="L4" s="40"/>
+      <c r="K4" s="90"/>
+      <c r="L4" s="91"/>
       <c r="M4" s="1"/>
       <c r="N4" s="1"/>
       <c r="O4" s="1"/>
       <c r="P4" s="1"/>
-      <c r="Q4" s="39"/>
-      <c r="R4" s="40"/>
+      <c r="Q4" s="90"/>
+      <c r="R4" s="91"/>
     </row>
     <row r="5" spans="5:18" x14ac:dyDescent="0.25">
       <c r="E5" s="1"/>
@@ -1615,14 +4063,14 @@
     </row>
     <row r="8" spans="5:18" x14ac:dyDescent="0.25">
       <c r="E8" s="1"/>
-      <c r="F8" s="48" t="s">
+      <c r="F8" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="G8" s="49"/>
-      <c r="H8" s="49"/>
-      <c r="I8" s="49"/>
-      <c r="J8" s="49"/>
-      <c r="K8" s="50"/>
+      <c r="G8" s="25"/>
+      <c r="H8" s="25"/>
+      <c r="I8" s="25"/>
+      <c r="J8" s="25"/>
+      <c r="K8" s="99"/>
       <c r="L8" s="2"/>
       <c r="M8" s="1"/>
       <c r="N8" s="1"/>
@@ -1633,12 +4081,12 @@
     </row>
     <row r="9" spans="5:18" x14ac:dyDescent="0.25">
       <c r="E9" s="1"/>
-      <c r="F9" s="48"/>
-      <c r="G9" s="49"/>
-      <c r="H9" s="49"/>
-      <c r="I9" s="49"/>
-      <c r="J9" s="49"/>
-      <c r="K9" s="50"/>
+      <c r="F9" s="24"/>
+      <c r="G9" s="25"/>
+      <c r="H9" s="25"/>
+      <c r="I9" s="25"/>
+      <c r="J9" s="25"/>
+      <c r="K9" s="99"/>
       <c r="L9" s="2"/>
       <c r="M9" s="1"/>
       <c r="N9" s="1"/>
@@ -1655,14 +4103,14 @@
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
       <c r="K10" s="1"/>
-      <c r="L10" s="48" t="s">
+      <c r="L10" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="M10" s="49"/>
-      <c r="N10" s="49"/>
-      <c r="O10" s="49"/>
-      <c r="P10" s="49"/>
-      <c r="Q10" s="50"/>
+      <c r="M10" s="25"/>
+      <c r="N10" s="25"/>
+      <c r="O10" s="25"/>
+      <c r="P10" s="25"/>
+      <c r="Q10" s="99"/>
       <c r="R10" s="2"/>
     </row>
     <row r="11" spans="5:18" x14ac:dyDescent="0.25">
@@ -1673,12 +4121,12 @@
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
       <c r="K11" s="1"/>
-      <c r="L11" s="48"/>
-      <c r="M11" s="49"/>
-      <c r="N11" s="49"/>
-      <c r="O11" s="49"/>
-      <c r="P11" s="49"/>
-      <c r="Q11" s="50"/>
+      <c r="L11" s="24"/>
+      <c r="M11" s="25"/>
+      <c r="N11" s="25"/>
+      <c r="O11" s="25"/>
+      <c r="P11" s="25"/>
+      <c r="Q11" s="99"/>
       <c r="R11" s="2"/>
     </row>
     <row r="12" spans="5:18" x14ac:dyDescent="0.25">
@@ -1721,36 +4169,36 @@
       <c r="X17" s="5"/>
     </row>
     <row r="18" spans="3:24" x14ac:dyDescent="0.25">
-      <c r="C18" s="11"/>
-      <c r="D18" s="12"/>
-      <c r="E18" s="41" t="s">
+      <c r="C18" s="76"/>
+      <c r="D18" s="77"/>
+      <c r="E18" s="92" t="s">
         <v>6</v>
       </c>
-      <c r="F18" s="42"/>
-      <c r="G18" s="42" t="s">
+      <c r="F18" s="93"/>
+      <c r="G18" s="93" t="s">
         <v>7</v>
       </c>
-      <c r="H18" s="42"/>
-      <c r="I18" s="42" t="s">
+      <c r="H18" s="93"/>
+      <c r="I18" s="93" t="s">
         <v>8</v>
       </c>
-      <c r="J18" s="42"/>
-      <c r="K18" s="42" t="s">
+      <c r="J18" s="93"/>
+      <c r="K18" s="93" t="s">
         <v>9</v>
       </c>
-      <c r="L18" s="42"/>
-      <c r="M18" s="42" t="s">
+      <c r="L18" s="93"/>
+      <c r="M18" s="93" t="s">
         <v>10</v>
       </c>
-      <c r="N18" s="45"/>
-      <c r="O18" s="47" t="s">
+      <c r="N18" s="96"/>
+      <c r="O18" s="98" t="s">
         <v>13</v>
       </c>
-      <c r="P18" s="17"/>
-      <c r="Q18" s="17" t="s">
+      <c r="P18" s="63"/>
+      <c r="Q18" s="63" t="s">
         <v>14</v>
       </c>
-      <c r="R18" s="17"/>
+      <c r="R18" s="63"/>
       <c r="T18" s="5"/>
       <c r="U18" s="5"/>
       <c r="V18" s="5"/>
@@ -1758,22 +4206,22 @@
       <c r="X18" s="5"/>
     </row>
     <row r="19" spans="3:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C19" s="13"/>
-      <c r="D19" s="14"/>
-      <c r="E19" s="43"/>
-      <c r="F19" s="44"/>
-      <c r="G19" s="44"/>
-      <c r="H19" s="44"/>
-      <c r="I19" s="44"/>
-      <c r="J19" s="44"/>
-      <c r="K19" s="44"/>
-      <c r="L19" s="44"/>
-      <c r="M19" s="44"/>
-      <c r="N19" s="46"/>
-      <c r="O19" s="47"/>
-      <c r="P19" s="17"/>
-      <c r="Q19" s="17"/>
-      <c r="R19" s="17"/>
+      <c r="C19" s="78"/>
+      <c r="D19" s="79"/>
+      <c r="E19" s="94"/>
+      <c r="F19" s="95"/>
+      <c r="G19" s="95"/>
+      <c r="H19" s="95"/>
+      <c r="I19" s="95"/>
+      <c r="J19" s="95"/>
+      <c r="K19" s="95"/>
+      <c r="L19" s="95"/>
+      <c r="M19" s="95"/>
+      <c r="N19" s="97"/>
+      <c r="O19" s="98"/>
+      <c r="P19" s="63"/>
+      <c r="Q19" s="63"/>
+      <c r="R19" s="63"/>
       <c r="T19" s="5"/>
       <c r="U19" s="5"/>
       <c r="V19" s="5"/>
@@ -1781,26 +4229,26 @@
       <c r="X19" s="5"/>
     </row>
     <row r="20" spans="3:24" x14ac:dyDescent="0.25">
-      <c r="C20" s="35" t="s">
+      <c r="C20" s="86" t="s">
         <v>11</v>
       </c>
-      <c r="D20" s="36"/>
-      <c r="E20" s="31">
+      <c r="D20" s="87"/>
+      <c r="E20" s="100">
         <v>0.13194444444444445</v>
       </c>
-      <c r="F20" s="32"/>
-      <c r="G20" s="33"/>
-      <c r="H20" s="33"/>
-      <c r="I20" s="32">
+      <c r="F20" s="73"/>
+      <c r="G20" s="74"/>
+      <c r="H20" s="74"/>
+      <c r="I20" s="73">
         <v>0.16666666666666666</v>
       </c>
-      <c r="J20" s="32"/>
-      <c r="K20" s="33"/>
-      <c r="L20" s="33"/>
-      <c r="M20" s="32">
+      <c r="J20" s="73"/>
+      <c r="K20" s="74"/>
+      <c r="L20" s="74"/>
+      <c r="M20" s="73">
         <v>0.16666666666666666</v>
       </c>
-      <c r="N20" s="34"/>
+      <c r="N20" s="75"/>
       <c r="Q20">
         <v>2</v>
       </c>
@@ -1813,18 +4261,18 @@
       <c r="X20" s="5"/>
     </row>
     <row r="21" spans="3:24" x14ac:dyDescent="0.25">
-      <c r="C21" s="27"/>
-      <c r="D21" s="28"/>
-      <c r="E21" s="21"/>
-      <c r="F21" s="19"/>
-      <c r="G21" s="24"/>
-      <c r="H21" s="24"/>
-      <c r="I21" s="19"/>
-      <c r="J21" s="19"/>
-      <c r="K21" s="24"/>
-      <c r="L21" s="24"/>
-      <c r="M21" s="19"/>
-      <c r="N21" s="20"/>
+      <c r="C21" s="82"/>
+      <c r="D21" s="83"/>
+      <c r="E21" s="67"/>
+      <c r="F21" s="65"/>
+      <c r="G21" s="70"/>
+      <c r="H21" s="70"/>
+      <c r="I21" s="65"/>
+      <c r="J21" s="65"/>
+      <c r="K21" s="70"/>
+      <c r="L21" s="70"/>
+      <c r="M21" s="65"/>
+      <c r="N21" s="66"/>
       <c r="T21" s="5"/>
       <c r="U21" s="5"/>
       <c r="V21" s="5"/>
@@ -1832,28 +4280,28 @@
       <c r="X21" s="5"/>
     </row>
     <row r="22" spans="3:24" x14ac:dyDescent="0.25">
-      <c r="C22" s="27" t="s">
+      <c r="C22" s="82" t="s">
         <v>12</v>
       </c>
-      <c r="D22" s="28"/>
-      <c r="E22" s="21">
+      <c r="D22" s="83"/>
+      <c r="E22" s="67">
         <v>0.10069444444444443</v>
       </c>
-      <c r="F22" s="19"/>
-      <c r="G22" s="24"/>
-      <c r="H22" s="24"/>
-      <c r="I22" s="19">
+      <c r="F22" s="65"/>
+      <c r="G22" s="70"/>
+      <c r="H22" s="70"/>
+      <c r="I22" s="65">
         <v>0.13194444444444445</v>
       </c>
-      <c r="J22" s="19"/>
-      <c r="K22" s="19">
+      <c r="J22" s="65"/>
+      <c r="K22" s="65">
         <v>0.13194444444444445</v>
       </c>
-      <c r="L22" s="19"/>
-      <c r="M22" s="19">
+      <c r="L22" s="65"/>
+      <c r="M22" s="65">
         <v>0.13194444444444445</v>
       </c>
-      <c r="N22" s="20"/>
+      <c r="N22" s="66"/>
       <c r="T22" s="5"/>
       <c r="U22" s="5"/>
       <c r="V22" s="5"/>
@@ -1861,18 +4309,18 @@
       <c r="X22" s="5"/>
     </row>
     <row r="23" spans="3:24" x14ac:dyDescent="0.25">
-      <c r="C23" s="27"/>
-      <c r="D23" s="28"/>
-      <c r="E23" s="21"/>
-      <c r="F23" s="19"/>
-      <c r="G23" s="24"/>
-      <c r="H23" s="24"/>
-      <c r="I23" s="19"/>
-      <c r="J23" s="19"/>
-      <c r="K23" s="19"/>
-      <c r="L23" s="19"/>
-      <c r="M23" s="19"/>
-      <c r="N23" s="20"/>
+      <c r="C23" s="82"/>
+      <c r="D23" s="83"/>
+      <c r="E23" s="67"/>
+      <c r="F23" s="65"/>
+      <c r="G23" s="70"/>
+      <c r="H23" s="70"/>
+      <c r="I23" s="65"/>
+      <c r="J23" s="65"/>
+      <c r="K23" s="65"/>
+      <c r="L23" s="65"/>
+      <c r="M23" s="65"/>
+      <c r="N23" s="66"/>
       <c r="T23" s="5"/>
       <c r="U23" s="5"/>
       <c r="V23" s="5"/>
@@ -1880,39 +4328,39 @@
       <c r="X23" s="5"/>
     </row>
     <row r="24" spans="3:24" x14ac:dyDescent="0.25">
-      <c r="C24" s="27" t="s">
+      <c r="C24" s="82" t="s">
         <v>13</v>
       </c>
-      <c r="D24" s="28"/>
-      <c r="E24" s="21">
+      <c r="D24" s="83"/>
+      <c r="E24" s="67">
         <f>E20+E22</f>
         <v>0.2326388888888889</v>
       </c>
-      <c r="F24" s="19"/>
-      <c r="G24" s="24"/>
-      <c r="H24" s="24"/>
-      <c r="I24" s="19">
+      <c r="F24" s="65"/>
+      <c r="G24" s="70"/>
+      <c r="H24" s="70"/>
+      <c r="I24" s="65">
         <v>0.30208333333333331</v>
       </c>
-      <c r="J24" s="19"/>
-      <c r="K24" s="19">
+      <c r="J24" s="65"/>
+      <c r="K24" s="65">
         <v>0.13194444444444445</v>
       </c>
-      <c r="L24" s="19"/>
-      <c r="M24" s="19">
+      <c r="L24" s="65"/>
+      <c r="M24" s="65">
         <v>0.30208333333333331</v>
       </c>
-      <c r="N24" s="20"/>
-      <c r="O24" s="15">
+      <c r="N24" s="66"/>
+      <c r="O24" s="80">
         <f>SUM(E24:N25)</f>
         <v>0.96875</v>
       </c>
-      <c r="P24" s="16"/>
-      <c r="Q24" s="18">
+      <c r="P24" s="81"/>
+      <c r="Q24" s="64">
         <f>O24*Q20</f>
         <v>1.9375</v>
       </c>
-      <c r="R24" s="18"/>
+      <c r="R24" s="64"/>
       <c r="T24" s="5"/>
       <c r="U24" s="5"/>
       <c r="V24" s="5"/>
@@ -1920,22 +4368,22 @@
       <c r="X24" s="5"/>
     </row>
     <row r="25" spans="3:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C25" s="29"/>
-      <c r="D25" s="30"/>
-      <c r="E25" s="22"/>
-      <c r="F25" s="23"/>
-      <c r="G25" s="25"/>
-      <c r="H25" s="25"/>
-      <c r="I25" s="23"/>
-      <c r="J25" s="23"/>
-      <c r="K25" s="23"/>
-      <c r="L25" s="23"/>
-      <c r="M25" s="23"/>
-      <c r="N25" s="26"/>
-      <c r="O25" s="15"/>
-      <c r="P25" s="16"/>
-      <c r="Q25" s="18"/>
-      <c r="R25" s="18"/>
+      <c r="C25" s="84"/>
+      <c r="D25" s="85"/>
+      <c r="E25" s="68"/>
+      <c r="F25" s="69"/>
+      <c r="G25" s="71"/>
+      <c r="H25" s="71"/>
+      <c r="I25" s="69"/>
+      <c r="J25" s="69"/>
+      <c r="K25" s="69"/>
+      <c r="L25" s="69"/>
+      <c r="M25" s="69"/>
+      <c r="N25" s="72"/>
+      <c r="O25" s="80"/>
+      <c r="P25" s="81"/>
+      <c r="Q25" s="64"/>
+      <c r="R25" s="64"/>
       <c r="T25" s="5"/>
       <c r="U25" s="5"/>
       <c r="V25" s="5"/>
@@ -1981,7 +4429,6 @@
     </row>
   </sheetData>
   <mergeCells count="35">
-    <mergeCell ref="C20:D21"/>
     <mergeCell ref="K3:L4"/>
     <mergeCell ref="E3:F4"/>
     <mergeCell ref="Q3:R4"/>
@@ -1995,13 +4442,13 @@
     <mergeCell ref="K8:K9"/>
     <mergeCell ref="Q10:Q11"/>
     <mergeCell ref="L10:P11"/>
+    <mergeCell ref="C18:D19"/>
+    <mergeCell ref="O24:P25"/>
+    <mergeCell ref="C22:D23"/>
+    <mergeCell ref="C24:D25"/>
+    <mergeCell ref="C20:D21"/>
     <mergeCell ref="E20:F21"/>
     <mergeCell ref="G20:H21"/>
-    <mergeCell ref="I20:J21"/>
-    <mergeCell ref="K20:L21"/>
-    <mergeCell ref="M20:N21"/>
-    <mergeCell ref="C18:D19"/>
-    <mergeCell ref="O24:P25"/>
     <mergeCell ref="Q18:R19"/>
     <mergeCell ref="Q24:R25"/>
     <mergeCell ref="M22:N23"/>
@@ -2010,12 +4457,13 @@
     <mergeCell ref="I24:J25"/>
     <mergeCell ref="K24:L25"/>
     <mergeCell ref="M24:N25"/>
-    <mergeCell ref="C22:D23"/>
-    <mergeCell ref="C24:D25"/>
     <mergeCell ref="E22:F23"/>
     <mergeCell ref="G22:H23"/>
     <mergeCell ref="I22:J23"/>
     <mergeCell ref="K22:L23"/>
+    <mergeCell ref="I20:J21"/>
+    <mergeCell ref="K20:L21"/>
+    <mergeCell ref="M20:N21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>